<commit_message>
[FIX]The error url of model
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="devops_app_template" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="devops_user" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t xml:space="preserve">devops_app_template</t>
   </si>
@@ -87,9 +88,19 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿微米黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">库</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">devops_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#gitlab_user_id</t>
   </si>
 </sst>
 </file>
@@ -105,6 +116,7 @@
       <color rgb="FF000000"/>
       <name val="文泉驿微米黑"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -120,13 +132,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DengXian"/>
-      <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <b val="true"/>
@@ -137,11 +142,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DengXian"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -169,7 +182,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,28 +209,20 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,15 +232,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="常规 2" xfId="22" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
@@ -246,7 +249,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A65536:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
@@ -254,12 +257,127 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2403433476395"/>
-    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="10.4463519313305"/>
-    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="10.6738197424893"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4635193133047"/>
+    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="15.2145922746781"/>
+    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="15.5579399141631"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="D7:J10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="15.2145922746781"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2961373390558"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.9184549356223"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.1587982832618"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="203.605150214592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.2532188841202"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.862660944206"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="15.2145922746781"/>
   </cols>
   <sheetData>
-    <row r="1048576" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -271,110 +389,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D7:J10"/>
+  <dimension ref="D7:F8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.4463519313305"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8712446351931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2489270386266"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2575107296137"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="136.038626609442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3948497854077"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5064377682403"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.4463519313305"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.1716738197425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6394849785408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1716738197425"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.9699570815451"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.1716738197425"/>
   </cols>
   <sheetData>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -382,8 +433,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"页 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ADD]the repository of Predefined template use githup
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -51,16 +51,16 @@
     <t xml:space="preserve">MicroService</t>
   </si>
   <si>
-    <t xml:space="preserve">app_template/MicroService.git</t>
+    <t xml:space="preserve">https://github.com/choerodon/choerodon-front-template.git</t>
   </si>
   <si>
     <t xml:space="preserve">微服务</t>
   </si>
   <si>
-    <t xml:space="preserve">MicroServiceUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app_template/MicroServiceUI.git</t>
+    <t xml:space="preserve">MicroServiceFront</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/choerodon/choerodon-microservice-template.git</t>
   </si>
   <si>
     <t xml:space="preserve">前端</t>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">JavaLib</t>
   </si>
   <si>
-    <t xml:space="preserve">app_template/JavaLib.git</t>
+    <t xml:space="preserve">https://github.com/choerodon/choerodon-javalib-template.git</t>
   </si>
   <si>
     <r>
@@ -257,9 +257,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4635193133047"/>
-    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="15.2145922746781"/>
-    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="15.5579399141631"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6223175965665"/>
+    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="17.2618025751073"/>
+    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="17.7167381974249"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -279,20 +279,20 @@
   </sheetPr>
   <dimension ref="D7:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="15.2145922746781"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2961373390558"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.9184549356223"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.1587982832618"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="203.605150214592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.2532188841202"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.862660944206"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="15.2145922746781"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="17.2618025751073"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4978540772532"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.7339055793991"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.8154506437768"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="233.017167381974"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.1158798283262"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.7424892703863"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="17.2618025751073"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -358,7 +358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
@@ -379,6 +379,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" display="https://github.com/choerodon/choerodon-front-template.git"/>
+    <hyperlink ref="G9" r:id="rId2" display="https://github.com/choerodon/choerodon-microservice-template.git"/>
+    <hyperlink ref="G10" r:id="rId3" display="https://github.com/choerodon/choerodon-javalib-template.git"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -402,11 +407,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.1716738197425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6394849785408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1716738197425"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.9699570815451"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.1716738197425"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.9914163090129"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.1630901287554"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9914163090129"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.6480686695279"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.9914163090129"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[ADD] modify the code of front template
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,21 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t xml:space="preserve">devops_app_template</t>
   </si>
   <si>
-    <t xml:space="preserve">*id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#name</t>
+    <t xml:space="preserve">#id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">repo_url</t>
   </si>
   <si>
-    <t xml:space="preserve">#code</t>
+    <t xml:space="preserve">code</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t xml:space="preserve">微服务</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MicroServiceUI</t>
   </si>
   <si>
     <t xml:space="preserve">MicroServiceFront</t>
@@ -93,17 +90,15 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">库</t>
+      <t xml:space="preserve">库
+</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">devops_user</t>
   </si>
   <si>
-    <t xml:space="preserve">#id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#gitlab_user_id</t>
+    <t xml:space="preserve">gitlab_user_id</t>
   </si>
 </sst>
 </file>
@@ -213,7 +208,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +227,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,9 +259,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2360515021459"/>
-    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="19.6437768240343"/>
-    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="9.08583690987125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.0042918454936"/>
+    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="18.1673819742489"/>
+    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="23.5064377682403"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -282,20 +281,20 @@
   </sheetPr>
   <dimension ref="D7:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="19.6437768240343"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.2660944206009"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.5708154506438"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.1502145922747"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="266.62660944206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5407725321888"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="45.3090128755365"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="19.6437768240343"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="18.1673819742489"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="104.017167381974"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="171.467811158798"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="117.643776824034"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="112.875536480687"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="96.9742489270386"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="123.321888412017"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="18.1673819742489"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,8 +321,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="2" t="s">
-        <v>7</v>
+      <c r="E8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>7</v>
@@ -342,40 +341,40 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>1</v>
@@ -403,28 +402,28 @@
   </sheetPr>
   <dimension ref="D7:F8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="17.0343347639485"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0214592274678"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0343347639485"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.1201716738197"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="17.0343347639485"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.0128755364807"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.3218884120172"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0128755364807"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="142.510729613734"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0128755364807"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,7 +431,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] init devops user
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="devops_app_template" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="devops_user" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t xml:space="preserve">devops_app_template</t>
   </si>
@@ -94,15 +93,6 @@
 </t>
     </r>
   </si>
-  <si>
-    <t xml:space="preserve">devops_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#iam_user_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gitlab_user_id</t>
-  </si>
 </sst>
 </file>
 
@@ -262,9 +252,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.9785407725322"/>
-    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="19.3047210300429"/>
-    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="25.0944206008584"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.1802575107296"/>
+    <col collapsed="false" hidden="false" max="1011" min="2" style="0" width="20.6652360515021"/>
+    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="26.7982832618026"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -284,20 +274,20 @@
   </sheetPr>
   <dimension ref="D7:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="19.3047210300429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="111.171673819742"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="183.390557939914"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="125.81974248927"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="120.708154506438"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="103.789699570815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="131.952789699571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="19.3047210300429"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="20.6652360515021"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="119.004291845494"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="196.223175965665"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="134.562231759657"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="129.111587982833"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="110.944206008584"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="141.150214592275"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="20.6652360515021"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,54 +386,4 @@
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="D7:F8"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.6952789699571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="93.343347639485"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6952789699571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="152.50643776824"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6952789699571"/>
-  </cols>
-  <sheetData>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,标准"页 &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[FIX] change init data groovy
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19770" windowHeight="8580" tabRatio="989" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8580" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>devops_app_template</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>is_synchro</t>
   </si>
   <si>
     <t>MicroService</t>
@@ -101,10 +104,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -141,16 +144,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,12 +180,41 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -176,86 +223,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,9 +248,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -282,10 +262,33 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -298,13 +301,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,31 +403,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,133 +481,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,8 +498,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,36 +524,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,6 +545,45 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -571,157 +592,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1078,10 +1081,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:J11"/>
+  <dimension ref="D7:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1096,7 +1099,7 @@
     <col min="10" max="1025" width="20.6666666666667"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:10">
+    <row r="7" spans="4:11">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1118,81 +1121,96 @@
       <c r="J7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="5:10">
+    <row r="8" spans="5:11">
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="I8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="5:10">
+    <row r="9" spans="5:11">
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" ht="30" spans="5:10">
+    <row r="10" ht="30" spans="5:11">
       <c r="E10" s="2">
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="6:10">
+    <row r="11" spans="6:11">
       <c r="F11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" t="s">
-        <v>16</v>
-      </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] fix init mocha teamplate
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>devops_app_template</t>
   </si>
   <si>
-    <t>#id</t>
+    <t>*id</t>
   </si>
   <si>
     <t>name</t>
@@ -33,7 +33,7 @@
     <t>repo_url</t>
   </si>
   <si>
-    <t>code</t>
+    <t>#code</t>
   </si>
   <si>
     <t>description</t>
@@ -83,7 +83,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="文泉驿微米黑"/>
-        <charset val="1"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">库
 </t>
@@ -104,12 +104,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -145,14 +145,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,33 +181,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -201,44 +194,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -247,6 +202,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -254,6 +224,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -276,6 +262,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -284,12 +277,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="文泉驿微米黑"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -301,187 +307,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,6 +498,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -514,21 +529,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -543,11 +543,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,136 +601,136 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1058,7 +1064,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1083,8 +1089,8 @@
   <sheetPr/>
   <dimension ref="D7:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E11 E9 E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1126,8 +1132,8 @@
       </c>
     </row>
     <row r="8" spans="5:11">
-      <c r="E8" s="2">
-        <v>1</v>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -1149,8 +1155,8 @@
       </c>
     </row>
     <row r="9" spans="5:11">
-      <c r="E9" s="2">
-        <v>2</v>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>11</v>
@@ -1172,8 +1178,8 @@
       </c>
     </row>
     <row r="10" ht="30" spans="5:11">
-      <c r="E10" s="2">
-        <v>3</v>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>14</v>
@@ -1194,7 +1200,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="6:11">
+    <row r="11" spans="5:11">
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
[ADD] add init app template data
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8580" tabRatio="989" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9347" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
   <si>
     <t>devops_app_template</t>
   </si>
@@ -98,6 +98,24 @@
   <si>
     <t>Mocha测试模板</t>
   </si>
+  <si>
+    <t>GoTemplate</t>
+  </si>
+  <si>
+    <t>https://github.com/choerodon/choerodon-golang-template</t>
+  </si>
+  <si>
+    <t>Go模板</t>
+  </si>
+  <si>
+    <t>SpringBootTemplate</t>
+  </si>
+  <si>
+    <t>https://github.com/choerodon/choerodon-springboot-template</t>
+  </si>
+  <si>
+    <t>SpringBoot模板</t>
+  </si>
 </sst>
 </file>
 
@@ -105,9 +123,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -151,8 +169,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -160,14 +241,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,16 +278,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,96 +307,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -307,67 +325,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,115 +493,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,29 +519,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,6 +549,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -554,21 +578,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,6 +599,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -601,199 +619,200 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -809,10 +828,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="212121"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F3F3F3"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1068,9 +1087,9 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="65.1777777777778"/>
+    <col min="1" max="1" width="65.175"/>
     <col min="2" max="1011" width="20.6666666666667"/>
     <col min="1012" max="1025" width="26.8"/>
   </cols>
@@ -1087,21 +1106,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:K11"/>
+  <dimension ref="D7:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E11 E9 E6:E9"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="3" width="20.6666666666667"/>
-    <col min="4" max="4" width="119.007407407407"/>
-    <col min="5" max="5" width="196.222222222222"/>
-    <col min="6" max="6" width="134.562962962963"/>
-    <col min="7" max="7" width="129.111111111111"/>
-    <col min="8" max="8" width="110.940740740741"/>
-    <col min="9" max="9" width="141.148148148148"/>
+    <col min="4" max="4" width="119.008333333333"/>
+    <col min="5" max="5" width="196.225"/>
+    <col min="6" max="6" width="134.566666666667"/>
+    <col min="7" max="7" width="129.108333333333"/>
+    <col min="8" max="8" width="110.941666666667"/>
+    <col min="9" max="9" width="141.15"/>
     <col min="10" max="1025" width="20.6666666666667"/>
   </cols>
   <sheetData>
@@ -1177,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="30" spans="5:11">
+    <row r="10" ht="31.2" spans="5:11">
       <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1190,7 +1209,7 @@
       <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J10">
@@ -1220,6 +1239,52 @@
         <v>1</v>
       </c>
       <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11">
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="5:11">
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <v>1</v>
       </c>
     </row>
@@ -1227,6 +1292,8 @@
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" display="https://github.com/choerodon/choerodon-microservice-template.git"/>
     <hyperlink ref="G10" r:id="rId2" display="https://github.com/choerodon/choerodon-javalib-template.git"/>
+    <hyperlink ref="G12" r:id="rId3" display="https://github.com/choerodon/choerodon-golang-template"/>
+    <hyperlink ref="G13" r:id="rId4" display="https://github.com/choerodon/choerodon-springboot-template"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
[IMP] change the logic of create app
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -102,7 +102,7 @@
     <t>GoTemplate</t>
   </si>
   <si>
-    <t>https://github.com/choerodon/choerodon-golang-template</t>
+    <t>https://github.com/choerodon/choerodon-golang-template.git</t>
   </si>
   <si>
     <t>Go模板</t>
@@ -111,7 +111,7 @@
     <t>SpringBootTemplate</t>
   </si>
   <si>
-    <t>https://github.com/choerodon/choerodon-springboot-template</t>
+    <t>https://github.com/choerodon/choerodon-springboot-template.git</t>
   </si>
   <si>
     <t>SpringBoot模板</t>
@@ -122,10 +122,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -162,40 +162,63 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -203,20 +226,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -224,24 +249,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,48 +280,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,6 +300,13 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,25 +325,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,31 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,61 +493,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,54 +506,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,21 +516,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -551,9 +536,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,21 +584,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -606,149 +593,162 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1108,8 +1108,8 @@
   <sheetPr/>
   <dimension ref="D7:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -1292,8 +1292,8 @@
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" display="https://github.com/choerodon/choerodon-microservice-template.git"/>
     <hyperlink ref="G10" r:id="rId2" display="https://github.com/choerodon/choerodon-javalib-template.git"/>
-    <hyperlink ref="G12" r:id="rId3" display="https://github.com/choerodon/choerodon-golang-template"/>
-    <hyperlink ref="G13" r:id="rId4" display="https://github.com/choerodon/choerodon-springboot-template"/>
+    <hyperlink ref="G12" r:id="rId3" display="https://github.com/choerodon/choerodon-golang-template.git" tooltip="https://github.com/choerodon/choerodon-golang-template.git"/>
+    <hyperlink ref="G13" r:id="rId4" display="https://github.com/choerodon/choerodon-springboot-template.git" tooltip="https://github.com/choerodon/choerodon-springboot-template.git"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
[ADD] add testng template
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-5-3-devops.xlsx
+++ b/src/main/resources/script/db/2018-5-3-devops.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
   <si>
     <t>devops_app_template</t>
   </si>
@@ -116,16 +116,25 @@
   <si>
     <t>SpringBoot模板</t>
   </si>
+  <si>
+    <t>ChoerodonTestngTemplate</t>
+  </si>
+  <si>
+    <t>https://github.com/choerodon/choerodon-testng-template.git</t>
+  </si>
+  <si>
+    <t>TestNg测试模板</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -162,11 +171,71 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -176,74 +245,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,16 +259,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,16 +281,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,9 +313,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,187 +334,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,27 +529,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,22 +562,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,6 +571,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -616,139 +610,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1106,10 +1115,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:K13"/>
+  <dimension ref="D7:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -1288,12 +1297,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="5:11">
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" display="https://github.com/choerodon/choerodon-microservice-template.git"/>
     <hyperlink ref="G10" r:id="rId2" display="https://github.com/choerodon/choerodon-javalib-template.git"/>
     <hyperlink ref="G12" r:id="rId3" display="https://github.com/choerodon/choerodon-golang-template.git" tooltip="https://github.com/choerodon/choerodon-golang-template.git"/>
     <hyperlink ref="G13" r:id="rId4" display="https://github.com/choerodon/choerodon-springboot-template.git" tooltip="https://github.com/choerodon/choerodon-springboot-template.git"/>
+    <hyperlink ref="G14" r:id="rId5" display="https://github.com/choerodon/choerodon-testng-template.git"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>